<commit_message>
maj feuille Excel (charges appartement: 2T 2017)
</commit_message>
<xml_diff>
--- a/Charges_appartement.xlsx
+++ b/Charges_appartement.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etienne\OpenClassrooms\Gérez code avec Git &amp; GitHub (cours)\Activites\activite1\work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etienne\OpenClassrooms\github\activite1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -707,7 +707,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,17 +845,19 @@
       <c r="B6" s="3">
         <v>662.16</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1">
+        <v>846.29</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="9"/>
       <c r="G6" s="12">
         <f t="shared" si="0"/>
-        <v>662.16</v>
+        <v>1508.4499999999998</v>
       </c>
       <c r="H6" s="13">
         <f t="shared" si="1"/>
-        <v>55.18</v>
+        <v>125.70416666666665</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
maj format feuilles Excel (ajout lignes années: 2020 à 2024)
</commit_message>
<xml_diff>
--- a/Charges_appartement.xlsx
+++ b/Charges_appartement.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Charges" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Charges!$A$1:$H$8</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Charges!$A$1:$H$13</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -119,7 +119,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -306,11 +306,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -364,6 +412,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -704,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,11 +893,11 @@
         <v>0</v>
       </c>
       <c r="G5" s="12">
-        <f t="shared" ref="G5:G8" si="0">SUM(B5:F5)</f>
+        <f t="shared" ref="G5:G13" si="0">SUM(B5:F5)</f>
         <v>3961.51</v>
       </c>
       <c r="H5" s="13">
-        <f t="shared" ref="H5:H8" si="1">G5/12</f>
+        <f t="shared" ref="H5:H13" si="1">G5/12</f>
         <v>330.12583333333333</v>
       </c>
     </row>
@@ -882,16 +945,106 @@
       <c r="A8" s="6">
         <v>2019</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="16">
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="22">
+        <f t="shared" ref="G8:G12" si="2">SUM(B8:F8)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="23">
+        <f t="shared" ref="H8:H12" si="3">G8/12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>2020</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>2021</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>2022</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>2024</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H13" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>